<commit_message>
Upload videos and update userIDs file
</commit_message>
<xml_diff>
--- a/userIDs.xlsx
+++ b/userIDs.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -18,15 +19,61 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+  <si>
+    <t>uID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>sID</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>2025-12-11</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,17 +93,117 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="3" builtinId="7"/>
+    <cellStyle name="Comma" xfId="4" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="5" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -330,13 +477,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1">
+      <c r="A2" s="1">
+        <v>66001</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1">
+      <c r="A3" s="1">
+        <v>66001</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1">
+      <c r="A4" s="1">
+        <v>66002</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add signal-fetcher.py script, add signal-fetcher.py instructions
</commit_message>
<xml_diff>
--- a/userIDs.xlsx
+++ b/userIDs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>uID</t>
   </si>
@@ -50,13 +50,22 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Database recording ID: 16ef52e7-8ae6-474c-8911-a6aec7bafe58</t>
+  </si>
+  <si>
+    <t>Database recording ID: 0565b6af-c324-47da-b684-458970d6e48c</t>
+  </si>
+  <si>
+    <t>Database recording ID: f565c08a-5fb8-41c5-9da7-e2a5dc1a6af8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +81,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -114,12 +129,24 @@
       <alignment/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -481,7 +508,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="topLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -503,7 +530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="1">
         <v>66001</v>
       </c>
@@ -516,22 +543,28 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1">
-      <c r="A3" s="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="3">
         <v>66001</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="1">
         <v>66002</v>
       </c>
@@ -543,6 +576,9 @@
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>